<commit_message>
software funcional hasta la ultima presentacion
</commit_message>
<xml_diff>
--- a/PlanStaffNewmont.xlsx
+++ b/PlanStaffNewmont.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -719,7 +719,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AWU15"/>
+  <dimension ref="A1:AWU16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -9142,6 +9142,53 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Vincent Rolong</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>KGB</t>
+        </is>
+      </c>
+      <c r="ARW16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARX16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARY16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ARZ16" s="22" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASA16" s="22" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+      <c r="ASB16" s="22" t="inlineStr">
+        <is>
+          <t>ON NS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
parcialmente funcional la logica de fechas report inbound outbound
</commit_message>
<xml_diff>
--- a/PlanStaffNewmont.xlsx
+++ b/PlanStaffNewmont.xlsx
@@ -9188,6 +9188,41 @@
           <t>ON NS</t>
         </is>
       </c>
+      <c r="ASD16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASE16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASF16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASG16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASH16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASI16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASJ16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
funcional 100% logica funcional en el reporte de inbound outbound 1009206928
</commit_message>
<xml_diff>
--- a/PlanStaffNewmont.xlsx
+++ b/PlanStaffNewmont.xlsx
@@ -49,7 +49,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill/>
     </fill>
@@ -108,6 +108,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFC7CE"/>
         <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFAA00"/>
+        <bgColor rgb="00FFAA00"/>
       </patternFill>
     </fill>
   </fills>
@@ -305,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -342,6 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,6 +423,36 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ShiftType</author>
+  </authors>
+  <commentList>
+    <comment ref="ASK16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASL16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASM16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASN16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9188,43 +9225,44 @@
           <t>ON NS</t>
         </is>
       </c>
-      <c r="ASD16" s="21" t="inlineStr">
+      <c r="ASH16" s="21" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ASE16" s="21" t="inlineStr">
+      <c r="ASI16" s="21" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ASF16" s="21" t="inlineStr">
+      <c r="ASJ16" s="21" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ASG16" s="21" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASH16" s="21" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASI16" s="21" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="ASJ16" s="21" t="inlineStr">
-        <is>
-          <t>ON</t>
+      <c r="ASK16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="ASL16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="ASM16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="ASN16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se solucionan errores de la version con recuperacion de BD el 11092025
</commit_message>
<xml_diff>
--- a/PlanStaffNewmont.xlsx
+++ b/PlanStaffNewmont.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -451,6 +451,41 @@
         <t>06:00-14:00</t>
       </text>
     </comment>
+    <comment ref="ASQ16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASR16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASS16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="AST16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASU16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASV16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
+    <comment ref="ASW16" authorId="0" shapeId="0">
+      <text>
+        <t>06:00-14:00</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -9260,6 +9295,41 @@
           <t>HD</t>
         </is>
       </c>
+      <c r="ASQ16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="ASR16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="ASS16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="AST16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="ASU16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="ASV16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="ASW16" s="24" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
codigo con mejora en la UI/UX pero necesita recuperar parte logica en relacion a la fechas que no corresponden a los cortes
</commit_message>
<xml_diff>
--- a/PlanStaffNewmont.xlsx
+++ b/PlanStaffNewmont.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -49,7 +49,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -114,6 +114,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFAA00"/>
         <bgColor rgb="00FFAA00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF3E88"/>
+        <bgColor rgb="00FF3E88"/>
       </patternFill>
     </fill>
   </fills>
@@ -311,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -349,6 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9330,6 +9337,26 @@
           <t>HD</t>
         </is>
       </c>
+      <c r="ASY16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ASZ16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATA16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="ATB16" s="21" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
interfaz visual ok faltsa testear full funcion
</commit_message>
<xml_diff>
--- a/PlanStaffNewmont.xlsx
+++ b/PlanStaffNewmont.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -7626,6 +7626,11 @@
           <t>Jonas Maceo</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NM00010</t>
+        </is>
+      </c>
       <c r="D11" s="1" t="n">
         <v>11</v>
       </c>

</xml_diff>